<commit_message>
sorted out template and EX_FILE
</commit_message>
<xml_diff>
--- a/Core/static/EnergyConsumptionDetail_updated.xlsx
+++ b/Core/static/EnergyConsumptionDetail_updated.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Customer 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,7 @@
     <sheet name="Customer 4" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Rate Price" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Example" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Sheet7" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Calculations" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="53">
   <si>
     <t xml:space="preserve">Customer Name</t>
   </si>
@@ -55,133 +55,121 @@
     <t xml:space="preserve">2nd Reading (kWh)</t>
   </si>
   <si>
-    <t xml:space="preserve">Consp Rate </t>
-  </si>
-  <si>
     <t xml:space="preserve">Day Rate</t>
   </si>
   <si>
     <t xml:space="preserve">Night Rate</t>
   </si>
   <si>
+    <t xml:space="preserve">Noel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2, Covent Garden, London</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YYYYYYYY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weekend Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martyn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3, Covent Garden, London</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XXXXXXXXX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weekday Day Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weekend Night Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vince</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4, Covent Garden, London</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WWWWWW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price (£/kWh)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weekend Day Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer Detail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate Detail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy Consumption = 2nd Reading - 1st Reading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XXX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flat X, London</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy Consumption for 'Rate 1' = 50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost for 'Rate 1' consumption = 50 * 0.5 = 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XYXYXYX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy Consumption for 'Rate 2' = 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost for 'Rate 2' consumption = 20 * 0.6 = 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy Consumption for 'Rate 3' = 60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost for 'Rate 3' consumption = 60 * 0.7 = 42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Energy Cost = 25 + 12 + 42 = 79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer Meter Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nighjt Rate</t>
+  </si>
+  <si>
     <t xml:space="preserve">Total Cost </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Noel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2, Covent Garden, London</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YYYYYYYY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total energy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weekend Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Martyn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3, Covent Garden, London</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XXXXXXXXX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weekday Day Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weekend Night Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vince</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4, Covent Garden, London</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WWWWWW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Energy </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Rate </t>
-  </si>
-  <si>
-    <t xml:space="preserve">None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price (£/kWh)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weekend Day Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Example </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customer Detail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rate Detail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calculation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy Consumption = 2nd Reading - 1st Reading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XXX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flat X, London</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rate 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy Consumption for 'Rate 1' = 50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost for 'Rate 1' consumption = 50 * 0.5 = 25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XYXYXYX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rate 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy Consumption for 'Rate 2' = 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost for 'Rate 2' consumption = 20 * 0.6 = 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rate 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy Consumption for 'Rate 3' = 60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost for 'Rate 3' consumption = 60 * 0.7 = 42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Energy Cost = 25 + 12 + 42 = 79</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customer Name </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customer Meter Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nighjt Rate</t>
   </si>
   <si>
     <t xml:space="preserve">joe</t>
@@ -495,7 +483,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -531,7 +519,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -542,13 +531,11 @@
         <v>8</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="0" t="s">
-        <v>9</v>
-      </c>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>3300</v>
@@ -556,16 +543,10 @@
       <c r="C6" s="0" t="n">
         <v>4500</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>1200</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>87.84</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>2300</v>
@@ -573,26 +554,14 @@
       <c r="C7" s="0" t="n">
         <v>2800</v>
       </c>
-      <c r="D7" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>27.5</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>115.34</v>
-      </c>
-    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -612,7 +581,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.671875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -622,7 +591,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -630,7 +599,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -638,10 +607,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -651,13 +620,11 @@
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1000</v>
@@ -665,16 +632,10 @@
       <c r="C6" s="0" t="n">
         <v>1600</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>43.92</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>2245</v>
@@ -682,16 +643,10 @@
       <c r="C7" s="0" t="n">
         <v>2350</v>
       </c>
-      <c r="D7" s="0" t="n">
-        <v>105</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>5.775</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>2850</v>
@@ -699,13 +654,11 @@
       <c r="C8" s="0" t="n">
         <v>3200</v>
       </c>
-      <c r="D8" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>0.945</v>
-      </c>
-    </row>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F16" s="1"/>
     </row>
@@ -728,7 +681,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -744,7 +697,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -752,7 +705,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -760,9 +713,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>6</v>
@@ -773,10 +727,12 @@
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>7150</v>
@@ -784,16 +740,10 @@
       <c r="C6" s="0" t="n">
         <v>7600</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>450</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>32.94</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>4365</v>
@@ -801,16 +751,10 @@
       <c r="C7" s="0" t="n">
         <v>4560</v>
       </c>
-      <c r="D7" s="0" t="n">
-        <v>195</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>10.725</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1977</v>
@@ -818,23 +762,14 @@
       <c r="C8" s="0" t="n">
         <v>2222</v>
       </c>
-      <c r="D8" s="0" t="n">
-        <v>245</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>15.435</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>58.1</v>
-      </c>
-    </row>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H20" s="1"/>
     </row>
@@ -856,8 +791,8 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -874,7 +809,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -882,7 +817,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -890,7 +825,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -903,16 +838,11 @@
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>44</v>
@@ -920,30 +850,21 @@
       <c r="C6" s="0" t="n">
         <v>900</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>856</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>62.6592</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1065</v>
@@ -951,23 +872,11 @@
       <c r="C8" s="0" t="n">
         <v>1430</v>
       </c>
-      <c r="D8" s="0" t="n">
-        <v>365</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>22.995</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>85.6542</v>
-      </c>
-    </row>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G17" s="1"/>
     </row>
@@ -1004,12 +913,12 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.0732</v>
@@ -1017,7 +926,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.055</v>
@@ -1025,7 +934,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.063</v>
@@ -1033,7 +942,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.067</v>
@@ -1041,7 +950,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.063</v>
@@ -1083,7 +992,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1091,18 +1000,18 @@
     </row>
     <row r="3" customFormat="false" ht="16.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="J4" s="0" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1110,13 +1019,13 @@
         <v>0</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
@@ -1127,19 +1036,19 @@
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G6" s="11" t="n">
         <v>0.5</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
@@ -1150,19 +1059,19 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G7" s="11" t="n">
         <v>0.6</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
@@ -1172,16 +1081,16 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="F8" s="15" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G8" s="16" t="n">
         <v>0.7</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1197,7 +1106,7 @@
     </row>
     <row r="10" customFormat="false" ht="16.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B10" s="6" t="n">
         <v>50</v>
@@ -1208,7 +1117,7 @@
     </row>
     <row r="11" customFormat="false" ht="16.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B11" s="6" t="n">
         <v>60</v>
@@ -1217,12 +1126,12 @@
         <v>80</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B12" s="20" t="n">
         <v>110</v>
@@ -1268,8 +1177,8 @@
   </sheetPr>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1285,18 +1194,18 @@
         <v>6</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>1</v>
@@ -1308,28 +1217,42 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
+      <c r="C4" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1200</v>
@@ -1337,7 +1260,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>600</v>
@@ -1345,7 +1268,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>450</v>
@@ -1353,7 +1276,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>856</v>
@@ -1361,7 +1284,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1374,7 +1297,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>105</v>
@@ -1382,7 +1305,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>195</v>
@@ -1390,7 +1313,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0</v>
@@ -1398,7 +1321,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>